<commit_message>
version 1.0.0 casi para salir a la cancha+
</commit_message>
<xml_diff>
--- a/archivosDefault/LD.xlsx
+++ b/archivosDefault/LD.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fboz\Desktop\generadorDeProyectos\archivosDefault\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0932E40-029C-4737-A10C-B5F61FBF9E56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18C76CCE-EF92-45E6-896D-1EE03C3140C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-5730" yWindow="-16320" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{D0A7AC39-8471-4F9C-83D3-27EFA39EA1BE}"/>
+    <workbookView xWindow="20370" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="1" xr2:uid="{D0A7AC39-8471-4F9C-83D3-27EFA39EA1BE}"/>
   </bookViews>
   <sheets>
     <sheet name="Carátula" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Listado de documentos'!$A$10:$G$10</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">Carátula!$A$1:$AP$60</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -28,19 +28,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="38">
   <si>
     <t>DOC. N°:</t>
   </si>
@@ -58,9 +51,6 @@
   </si>
   <si>
     <t>A</t>
-  </si>
-  <si>
-    <t>2 de 2</t>
   </si>
   <si>
     <t>FECHA</t>
@@ -1725,8 +1715,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A628930B-8D02-4543-A186-798CC476F41A}">
   <dimension ref="B1:AO135"/>
   <sheetViews>
-    <sheetView showGridLines="0" view="pageBreakPreview" topLeftCell="A33" zoomScale="130" zoomScaleNormal="55" zoomScaleSheetLayoutView="130" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="BF47" sqref="BF47"/>
+    <sheetView showGridLines="0" view="pageBreakPreview" topLeftCell="A42" zoomScale="130" zoomScaleNormal="55" zoomScaleSheetLayoutView="130" zoomScalePageLayoutView="70" workbookViewId="0">
+      <selection activeCell="F57" sqref="F57:P58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="1.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1783,7 +1773,7 @@
       <c r="C3" s="14"/>
       <c r="E3" s="1"/>
       <c r="F3" s="80" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G3" s="81"/>
       <c r="H3" s="81"/>
@@ -3668,13 +3658,13 @@
       <c r="C49" s="14"/>
       <c r="E49" s="1"/>
       <c r="F49" s="89" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G49" s="90"/>
       <c r="H49" s="46"/>
       <c r="I49" s="47"/>
       <c r="J49" s="48" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="K49" s="49"/>
       <c r="L49" s="50"/>
@@ -3682,7 +3672,7 @@
       <c r="N49" s="74"/>
       <c r="O49" s="75"/>
       <c r="P49" s="24" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="Q49" s="25"/>
       <c r="R49" s="25"/>
@@ -3694,29 +3684,29 @@
       <c r="X49" s="25"/>
       <c r="Y49" s="26"/>
       <c r="Z49" s="27" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="AA49" s="46" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="AB49" s="53"/>
       <c r="AC49" s="53"/>
       <c r="AD49" s="53"/>
       <c r="AE49" s="47"/>
       <c r="AF49" s="46" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="AG49" s="47"/>
       <c r="AH49" s="46" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="AI49" s="47"/>
       <c r="AJ49" s="46" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="AK49" s="47"/>
       <c r="AL49" s="46" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="AM49" s="53"/>
       <c r="AN49" s="47"/>
@@ -3727,13 +3717,13 @@
       <c r="C50" s="17"/>
       <c r="E50" s="1"/>
       <c r="F50" s="89" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G50" s="90"/>
       <c r="H50" s="46"/>
       <c r="I50" s="47"/>
       <c r="J50" s="51" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="K50" s="49"/>
       <c r="L50" s="50"/>
@@ -3751,25 +3741,25 @@
       <c r="X50" s="29"/>
       <c r="Y50" s="30"/>
       <c r="Z50" s="27" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="AA50" s="46" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="AB50" s="53"/>
       <c r="AC50" s="53"/>
       <c r="AD50" s="53"/>
       <c r="AE50" s="47"/>
       <c r="AF50" s="46" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="AG50" s="47"/>
       <c r="AH50" s="46" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="AI50" s="47"/>
       <c r="AJ50" s="46" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="AK50" s="47"/>
       <c r="AL50" s="52"/>
@@ -3782,13 +3772,13 @@
       <c r="C51" s="14"/>
       <c r="E51" s="1"/>
       <c r="F51" s="89" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G51" s="90"/>
       <c r="H51" s="46"/>
       <c r="I51" s="47"/>
       <c r="J51" s="51" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="K51" s="49"/>
       <c r="L51" s="50"/>
@@ -3809,7 +3799,7 @@
         <v>5</v>
       </c>
       <c r="AA51" s="76" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="AB51" s="77"/>
       <c r="AC51" s="77"/>
@@ -3831,13 +3821,13 @@
       <c r="C52" s="17"/>
       <c r="E52" s="1"/>
       <c r="F52" s="89" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G52" s="90"/>
       <c r="H52" s="46"/>
       <c r="I52" s="47"/>
       <c r="J52" s="51" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="K52" s="49"/>
       <c r="L52" s="50"/>
@@ -3858,26 +3848,26 @@
         <v>1</v>
       </c>
       <c r="AA52" s="51" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="AB52" s="49"/>
       <c r="AC52" s="49"/>
       <c r="AD52" s="49"/>
       <c r="AE52" s="50"/>
       <c r="AF52" s="51" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="AG52" s="50"/>
       <c r="AH52" s="51" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="AI52" s="50"/>
       <c r="AJ52" s="51" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="AK52" s="50"/>
       <c r="AL52" s="51" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="AM52" s="49"/>
       <c r="AN52" s="50"/>
@@ -3888,7 +3878,7 @@
       <c r="C53" s="14"/>
       <c r="E53" s="1"/>
       <c r="F53" s="71" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G53" s="72"/>
       <c r="H53" s="72"/>
@@ -3918,12 +3908,12 @@
       <c r="AF53" s="92"/>
       <c r="AG53" s="93"/>
       <c r="AH53" s="59" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="AI53" s="60"/>
       <c r="AJ53" s="61"/>
       <c r="AK53" s="71" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="AL53" s="72"/>
       <c r="AM53" s="35"/>
@@ -3966,7 +3956,7 @@
       <c r="AI54" s="63"/>
       <c r="AJ54" s="64"/>
       <c r="AK54" s="65" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="AL54" s="66"/>
       <c r="AM54" s="66"/>
@@ -3987,8 +3977,9 @@
       <c r="M55" s="29"/>
       <c r="N55" s="29"/>
       <c r="O55" s="30"/>
-      <c r="P55" s="91" t="s">
-        <v>31</v>
+      <c r="P55" s="91" t="str">
+        <f>F3</f>
+        <v>Listado de documentos</v>
       </c>
       <c r="Q55" s="92"/>
       <c r="R55" s="92"/>
@@ -4011,7 +4002,7 @@
       <c r="AI55" s="63"/>
       <c r="AJ55" s="64"/>
       <c r="AK55" s="71" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="AL55" s="72"/>
       <c r="AM55" s="72"/>
@@ -4051,12 +4042,12 @@
       <c r="AF56" s="95"/>
       <c r="AG56" s="96"/>
       <c r="AH56" s="54" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="AI56" s="55"/>
       <c r="AJ56" s="56"/>
       <c r="AK56" s="65" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="AL56" s="66"/>
       <c r="AM56" s="66"/>
@@ -4068,7 +4059,7 @@
       <c r="C57" s="14"/>
       <c r="E57" s="1"/>
       <c r="F57" s="97" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G57" s="81"/>
       <c r="H57" s="81"/>
@@ -4098,14 +4089,14 @@
       <c r="AF57" s="99"/>
       <c r="AG57" s="100"/>
       <c r="AH57" s="22" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="AI57" s="57" t="s">
         <v>5</v>
       </c>
       <c r="AJ57" s="19"/>
       <c r="AK57" s="22" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="AL57" s="18"/>
       <c r="AM57" s="18"/>
@@ -4340,7 +4331,7 @@
   <dimension ref="A1:S38"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="70" workbookViewId="0">
-      <selection activeCell="I21" sqref="I21"/>
+      <selection activeCell="I5" sqref="I5:I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4365,14 +4356,18 @@
       <c r="D1" s="116" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="119"/>
+      <c r="E1" s="119">
+        <f>Carátula!Q57</f>
+        <v>0</v>
+      </c>
       <c r="F1" s="120"/>
       <c r="G1" s="120"/>
       <c r="H1" s="104" t="s">
         <v>1</v>
       </c>
-      <c r="I1" s="104" t="s">
-        <v>5</v>
+      <c r="I1" s="104" t="str">
+        <f>Carátula!AI57</f>
+        <v>A</v>
       </c>
     </row>
     <row r="2" spans="1:19" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -4415,15 +4410,16 @@
       <c r="D5" s="116" t="s">
         <v>2</v>
       </c>
-      <c r="E5" s="119"/>
+      <c r="E5" s="119" t="str">
+        <f>Carátula!P55</f>
+        <v>Listado de documentos</v>
+      </c>
       <c r="F5" s="120"/>
       <c r="G5" s="120"/>
       <c r="H5" s="104" t="s">
         <v>3</v>
       </c>
-      <c r="I5" s="107" t="s">
-        <v>6</v>
-      </c>
+      <c r="I5" s="107"/>
     </row>
     <row r="6" spans="1:19" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="112"/>
@@ -4472,22 +4468,22 @@
         <v>4</v>
       </c>
       <c r="B10" s="38" t="s">
+        <v>31</v>
+      </c>
+      <c r="C10" s="38" t="s">
         <v>32</v>
       </c>
-      <c r="C10" s="38" t="s">
+      <c r="D10" s="39" t="s">
         <v>33</v>
       </c>
-      <c r="D10" s="39" t="s">
+      <c r="E10" s="39" t="s">
         <v>34</v>
       </c>
-      <c r="E10" s="39" t="s">
+      <c r="F10" s="38" t="s">
         <v>35</v>
       </c>
-      <c r="F10" s="38" t="s">
+      <c r="G10" s="39" t="s">
         <v>36</v>
-      </c>
-      <c r="G10" s="39" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="11" spans="1:19" s="11" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>